<commit_message>
Auswertung mizt rawDataA, B
Motorimpulse invertiert.
</commit_message>
<xml_diff>
--- a/PORT-Belegung DEcoder.xlsx
+++ b/PORT-Belegung DEcoder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Elektronik/ AVR/ AVR_Programme/AVR HomeCentral/Slave/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Elektronik/ AVR/ AVR_Programme/H0_Decoder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DE35DB2-C91A-9740-87ED-EFB653A13A3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6C793C-4266-3C4D-8F85-757A02648891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="29260" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="16000" yWindow="29260" windowWidth="13580" windowHeight="14840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heizung" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <sheet name="SPI_Strom" sheetId="2" r:id="rId9"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="108">
   <si>
     <t>Portbelegung</t>
   </si>
@@ -162,13 +162,7 @@
   </si>
   <si>
     <t>D0</t>
-  </si>
-  <si>
-    <t>D0</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>D1</t>
   </si>
   <si>
     <t>D1</t>
@@ -176,13 +170,7 @@
   </si>
   <si>
     <t>D2</t>
-  </si>
-  <si>
-    <t>D2</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>D3</t>
   </si>
   <si>
     <t>D3</t>
@@ -190,13 +178,7 @@
   </si>
   <si>
     <t>C0</t>
-  </si>
-  <si>
-    <t>C0</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C1</t>
   </si>
   <si>
     <t>C1</t>
@@ -204,93 +186,17 @@
   </si>
   <si>
     <t>C2</t>
-  </si>
-  <si>
-    <t>C2</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C3</t>
   </si>
   <si>
     <t>C3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Uhr EIN</t>
-  </si>
-  <si>
-    <t>Uhr AUS</t>
-  </si>
-  <si>
-    <t>Rinne EIN</t>
-  </si>
-  <si>
-    <t>Rinne AUS</t>
-  </si>
-  <si>
     <t>Manuell</t>
   </si>
   <si>
     <t>D5</t>
-  </si>
-  <si>
-    <t>ADC Vorlauf</t>
-  </si>
-  <si>
-    <t>ADC Rücklauf</t>
-  </si>
-  <si>
-    <t>ADC Aussen</t>
-  </si>
-  <si>
-    <t>ADC Tastatur</t>
-  </si>
-  <si>
-    <t>Taste 0</t>
-  </si>
-  <si>
-    <t>B0</t>
-  </si>
-  <si>
-    <t>Servo A</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>Brenner Status</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>Servo A (OC1A)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Servo B (OC1B)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UHREIN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UHRAUS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RINNEEIN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RINNEAUS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MANUELL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LCD_RSDS</t>
@@ -305,31 +211,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CONTROL_A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>OSZIA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADC Vorlauf</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADC Aussen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADC Tastatur</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eingang Brennerstatus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heizung</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -474,16 +356,46 @@
     <t>FIRSTRUN</t>
   </si>
   <si>
-    <t>DS1820</t>
+    <t>MOTOROUT</t>
   </si>
   <si>
-    <t>B3</t>
+    <t>MOTOEDIR</t>
+  </si>
+  <si>
+    <t>FUNKTIONOK</t>
+  </si>
+  <si>
+    <t>ADDRESSOK</t>
+  </si>
+  <si>
+    <t>DATAOK</t>
+  </si>
+  <si>
+    <t>TEST1</t>
+  </si>
+  <si>
+    <t>TEST2</t>
+  </si>
+  <si>
+    <t>TEST0</t>
+  </si>
+  <si>
+    <t>PAKETA</t>
+  </si>
+  <si>
+    <t>PAKETB</t>
+  </si>
+  <si>
+    <t>FUNKTION</t>
+  </si>
+  <si>
+    <t>H0-Decoder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -518,11 +430,6 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
       <sz val="14"/>
       <name val="Verdana"/>
     </font>
@@ -535,6 +442,12 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -763,22 +676,21 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -796,6 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2174,11 +2087,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG24" sqref="AG24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2196,18 +2110,18 @@
     <col min="31" max="31" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="46" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
+    <row r="1" spans="1:29" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>107</v>
       </c>
       <c r="B1" s="17"/>
     </row>
-    <row r="2" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" s="19" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D3" s="20" t="str">
         <f>IF(COUNTA(D7:D222)&gt;1,"x","")</f>
         <v/>
@@ -2310,7 +2224,7 @@
       </c>
       <c r="AC3" s="21"/>
     </row>
-    <row r="4" spans="1:31" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D4" s="18">
         <f>COUNTA(D7:D61)</f>
         <v>1</v>
@@ -2325,7 +2239,7 @@
       </c>
       <c r="G4" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="18">
         <f t="shared" si="1"/>
@@ -2350,7 +2264,7 @@
       </c>
       <c r="N4" s="18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="18">
         <f t="shared" si="1"/>
@@ -2366,11 +2280,11 @@
       </c>
       <c r="R4" s="18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="18">
         <f t="shared" si="1"/>
@@ -2394,7 +2308,7 @@
       </c>
       <c r="Y4" s="18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="18">
         <f t="shared" si="1"/>
@@ -2410,7 +2324,7 @@
       </c>
       <c r="AC4" s="11"/>
     </row>
-    <row r="5" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D5" s="34" t="s">
         <v>1</v>
       </c>
@@ -2442,7 +2356,7 @@
       <c r="AB5" s="36"/>
       <c r="AC5" s="37"/>
     </row>
-    <row r="6" spans="1:31" s="38" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" s="38" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="D6" s="39">
         <v>7</v>
       </c>
@@ -2514,982 +2428,906 @@
       </c>
       <c r="AC6" s="44"/>
     </row>
-    <row r="7" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="33">
         <f>IF(SUM(D7:AB7)=0,0,SUM(D7:AB7))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="48"/>
-      <c r="U7" s="51"/>
-      <c r="V7" s="51"/>
-      <c r="W7" s="51"/>
-      <c r="X7" s="51"/>
-      <c r="Y7" s="51"/>
-      <c r="Z7" s="51"/>
-      <c r="AA7" s="51"/>
-      <c r="AB7" s="51"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="50"/>
+      <c r="X7" s="50"/>
+      <c r="Y7" s="50"/>
+      <c r="Z7" s="50"/>
+      <c r="AA7" s="50"/>
+      <c r="AB7" s="50"/>
       <c r="AC7" s="44"/>
-      <c r="AD7" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE7" s="33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="33">
         <f t="shared" ref="A8:A55" si="2">IF(SUM(D8:AB8)=0,0,SUM(D8:AB8))</f>
-        <v>1</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47">
-        <v>1</v>
-      </c>
-      <c r="K8" s="47"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="50"/>
+      <c r="AA8" s="50"/>
+      <c r="AB8" s="52"/>
       <c r="AC8" s="44"/>
-      <c r="AD8" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE8" s="33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="51"/>
-      <c r="X9" s="51"/>
-      <c r="Y9" s="51"/>
-      <c r="Z9" s="51"/>
-      <c r="AA9" s="51"/>
-      <c r="AB9" s="53"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="50"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="50"/>
+      <c r="X9" s="50"/>
+      <c r="Y9" s="50"/>
+      <c r="Z9" s="50"/>
+      <c r="AA9" s="50"/>
+      <c r="AB9" s="52"/>
       <c r="AC9" s="44"/>
-      <c r="AD9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE9" s="33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="51"/>
-      <c r="V10" s="51"/>
-      <c r="W10" s="51"/>
-      <c r="X10" s="51"/>
-      <c r="Y10" s="51"/>
-      <c r="Z10" s="51"/>
-      <c r="AA10" s="51"/>
-      <c r="AB10" s="53"/>
+        <v>1</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49">
+        <v>1</v>
+      </c>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="50"/>
+      <c r="V10" s="50"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="50"/>
+      <c r="Y10" s="50"/>
+      <c r="Z10" s="50"/>
+      <c r="AA10" s="50"/>
+      <c r="AB10" s="52"/>
       <c r="AC10" s="44"/>
-      <c r="AD10" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE10" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="50"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="51"/>
-      <c r="V11" s="51"/>
-      <c r="W11" s="51"/>
-      <c r="X11" s="51"/>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="51"/>
-      <c r="AA11" s="51"/>
-      <c r="AB11" s="53">
-        <v>1</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="50"/>
+      <c r="AA11" s="50"/>
+      <c r="AB11" s="52"/>
       <c r="AC11" s="44"/>
-      <c r="AD11" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE11" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="51"/>
-      <c r="V12" s="51"/>
-      <c r="W12" s="51"/>
-      <c r="X12" s="51"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="51"/>
-      <c r="AA12" s="51">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="53"/>
+        <v>100</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49">
+        <v>1</v>
+      </c>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="52"/>
       <c r="AC12" s="44"/>
     </row>
-    <row r="13" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="51"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="51"/>
-      <c r="AA13" s="51"/>
-      <c r="AB13" s="53"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="52"/>
       <c r="AC13" s="44"/>
     </row>
-    <row r="14" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50"/>
-      <c r="T14" s="52"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="51">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="51"/>
-      <c r="AB14" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="50"/>
+      <c r="AA14" s="50"/>
+      <c r="AB14" s="52"/>
       <c r="AC14" s="44"/>
     </row>
-    <row r="15" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="52"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="51">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="51"/>
-      <c r="AA15" s="51"/>
-      <c r="AB15" s="53"/>
+        <v>103</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46">
+        <v>1</v>
+      </c>
+      <c r="L15" s="51"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="50"/>
+      <c r="X15" s="50"/>
+      <c r="Y15" s="50"/>
+      <c r="Z15" s="50"/>
+      <c r="AA15" s="50"/>
+      <c r="AB15" s="52"/>
       <c r="AC15" s="44"/>
-      <c r="AD15" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE15" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
-      <c r="T16" s="52"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="51"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="51"/>
-      <c r="Y16" s="51"/>
-      <c r="Z16" s="51"/>
-      <c r="AA16" s="51"/>
-      <c r="AB16" s="53"/>
+        <v>1</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46">
+        <v>1</v>
+      </c>
+      <c r="K16" s="46"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="50"/>
+      <c r="V16" s="50"/>
+      <c r="W16" s="50"/>
+      <c r="X16" s="50"/>
+      <c r="Y16" s="50"/>
+      <c r="Z16" s="50"/>
+      <c r="AA16" s="50"/>
+      <c r="AB16" s="52"/>
       <c r="AC16" s="44"/>
-      <c r="AD16" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE16" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="50"/>
-      <c r="S17" s="50"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51">
-        <v>1</v>
-      </c>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="51"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="53"/>
+        <v>102</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46">
+        <v>1</v>
+      </c>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="52"/>
       <c r="AC17" s="44"/>
-      <c r="AD17" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE17" s="33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="50"/>
-      <c r="S18" s="50"/>
-      <c r="T18" s="52"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="51"/>
-      <c r="Z18" s="51"/>
-      <c r="AA18" s="51"/>
-      <c r="AB18" s="53"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="52"/>
       <c r="AC18" s="44"/>
-      <c r="AD18" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE18" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="50"/>
-      <c r="S19" s="50"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="51"/>
-      <c r="Z19" s="51"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="53"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="50"/>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="52"/>
       <c r="AC19" s="44"/>
     </row>
-    <row r="20" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="50"/>
-      <c r="S20" s="50"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="51"/>
-      <c r="V20" s="51"/>
-      <c r="W20" s="51"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="51"/>
-      <c r="Z20" s="51"/>
-      <c r="AA20" s="51"/>
-      <c r="AB20" s="53"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="52"/>
       <c r="AC20" s="44"/>
     </row>
-    <row r="21" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47">
-        <v>1</v>
-      </c>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="50"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="51"/>
-      <c r="AA21" s="51"/>
-      <c r="AB21" s="53"/>
+        <v>45</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46">
+        <v>1</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="50"/>
+      <c r="AB21" s="52"/>
       <c r="AC21" s="44"/>
-      <c r="AD21" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE21" s="33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47">
-        <v>1</v>
-      </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="50"/>
-      <c r="R22" s="50"/>
-      <c r="S22" s="50"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="53"/>
+        <v>46</v>
+      </c>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46">
+        <v>1</v>
+      </c>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="49"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="50"/>
+      <c r="V22" s="50"/>
+      <c r="W22" s="50"/>
+      <c r="X22" s="50"/>
+      <c r="Y22" s="50"/>
+      <c r="Z22" s="50"/>
+      <c r="AA22" s="50"/>
+      <c r="AB22" s="52"/>
       <c r="AC22" s="44"/>
-      <c r="AD22" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE22" s="33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="47">
-        <v>1</v>
-      </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="50"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="51"/>
-      <c r="Z23" s="51"/>
-      <c r="AA23" s="51"/>
-      <c r="AB23" s="53"/>
+        <v>47</v>
+      </c>
+      <c r="D23" s="46">
+        <v>1</v>
+      </c>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="51"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="50"/>
+      <c r="X23" s="50"/>
+      <c r="Y23" s="50"/>
+      <c r="Z23" s="50"/>
+      <c r="AA23" s="50"/>
+      <c r="AB23" s="52"/>
       <c r="AC23" s="44"/>
-      <c r="AD23" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE23" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="50"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="50"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="51"/>
-      <c r="Z24" s="51"/>
-      <c r="AA24" s="51"/>
-      <c r="AB24" s="53"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="50"/>
+      <c r="Z24" s="50"/>
+      <c r="AA24" s="50"/>
+      <c r="AB24" s="52"/>
       <c r="AC24" s="44"/>
-      <c r="AD24" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE24" s="33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="50"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="50"/>
-      <c r="T25" s="52"/>
-      <c r="U25" s="51"/>
-      <c r="V25" s="51">
-        <v>1</v>
-      </c>
-      <c r="W25" s="51"/>
-      <c r="X25" s="51"/>
-      <c r="Y25" s="51"/>
-      <c r="Z25" s="51"/>
-      <c r="AA25" s="51"/>
-      <c r="AB25" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="50"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="50"/>
+      <c r="Z25" s="50"/>
+      <c r="AA25" s="50"/>
+      <c r="AB25" s="52"/>
       <c r="AC25" s="44"/>
     </row>
-    <row r="26" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="50"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="50"/>
-      <c r="R26" s="50"/>
-      <c r="S26" s="50"/>
-      <c r="T26" s="52"/>
-      <c r="U26" s="51">
-        <v>1</v>
-      </c>
-      <c r="V26" s="51"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="51"/>
-      <c r="Z26" s="51"/>
-      <c r="AA26" s="51"/>
-      <c r="AB26" s="53"/>
+        <v>48</v>
+      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50">
+        <v>1</v>
+      </c>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="50"/>
+      <c r="AA26" s="50"/>
+      <c r="AB26" s="52"/>
       <c r="AC26" s="44"/>
     </row>
-    <row r="27" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="52"/>
-      <c r="U27" s="51"/>
-      <c r="V27" s="51"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="51"/>
-      <c r="Y27" s="51"/>
-      <c r="Z27" s="51"/>
-      <c r="AA27" s="51"/>
-      <c r="AB27" s="53"/>
+        <v>1</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="51"/>
+      <c r="U27" s="50">
+        <v>1</v>
+      </c>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="50"/>
+      <c r="Z27" s="50"/>
+      <c r="AA27" s="50"/>
+      <c r="AB27" s="52"/>
       <c r="AC27" s="44"/>
     </row>
-    <row r="28" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="51"/>
-      <c r="Z28" s="51"/>
-      <c r="AA28" s="51"/>
-      <c r="AB28" s="53"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="50"/>
+      <c r="AA28" s="50"/>
+      <c r="AB28" s="52"/>
       <c r="AC28" s="44"/>
     </row>
-    <row r="29" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47">
-        <v>1</v>
-      </c>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="50"/>
-      <c r="O29" s="50"/>
-      <c r="P29" s="50"/>
-      <c r="Q29" s="50"/>
-      <c r="R29" s="50"/>
-      <c r="S29" s="50"/>
-      <c r="T29" s="52"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="51"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="51"/>
-      <c r="Z29" s="51"/>
-      <c r="AA29" s="51"/>
-      <c r="AB29" s="53"/>
+        <v>68</v>
+      </c>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="50">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="50"/>
+      <c r="AB29" s="52"/>
       <c r="AC29" s="44"/>
     </row>
-    <row r="30" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="50"/>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="50"/>
-      <c r="T30" s="52"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="51"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="51"/>
-      <c r="AA30" s="51"/>
-      <c r="AB30" s="53"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="50"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="52"/>
       <c r="AC30" s="44"/>
     </row>
-    <row r="31" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="51"/>
-      <c r="W31" s="51"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="51"/>
-      <c r="Z31" s="51"/>
-      <c r="AA31" s="51"/>
-      <c r="AB31" s="53"/>
+        <v>1</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46">
+        <v>1</v>
+      </c>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="50"/>
+      <c r="V31" s="50"/>
+      <c r="W31" s="50"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="50"/>
+      <c r="Z31" s="50"/>
+      <c r="AA31" s="50"/>
+      <c r="AB31" s="52"/>
       <c r="AC31" s="44"/>
     </row>
-    <row r="32" spans="1:31" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47">
-        <v>1</v>
-      </c>
-      <c r="L32" s="52"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="51"/>
-      <c r="W32" s="51"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="51"/>
-      <c r="Z32" s="51"/>
-      <c r="AA32" s="51"/>
-      <c r="AB32" s="53"/>
+        <v>97</v>
+      </c>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46">
+        <v>1</v>
+      </c>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="51"/>
+      <c r="U32" s="50"/>
+      <c r="V32" s="50"/>
+      <c r="W32" s="50"/>
+      <c r="X32" s="50"/>
+      <c r="Y32" s="50"/>
+      <c r="Z32" s="50"/>
+      <c r="AA32" s="50"/>
+      <c r="AB32" s="52"/>
       <c r="AC32" s="44"/>
     </row>
     <row r="33" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3497,34 +3335,31 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="B33" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="50"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="51"/>
-      <c r="V33" s="51"/>
-      <c r="W33" s="51"/>
-      <c r="X33" s="51"/>
-      <c r="Y33" s="51"/>
-      <c r="Z33" s="51"/>
-      <c r="AA33" s="51"/>
-      <c r="AB33" s="53"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="50"/>
+      <c r="V33" s="50"/>
+      <c r="W33" s="50"/>
+      <c r="X33" s="50"/>
+      <c r="Y33" s="50"/>
+      <c r="Z33" s="50"/>
+      <c r="AA33" s="50"/>
+      <c r="AB33" s="52"/>
       <c r="AC33" s="44"/>
     </row>
     <row r="34" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3532,63 +3367,68 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50"/>
-      <c r="T34" s="52"/>
-      <c r="U34" s="51"/>
-      <c r="V34" s="51"/>
-      <c r="W34" s="51"/>
-      <c r="X34" s="51"/>
-      <c r="Y34" s="51"/>
-      <c r="Z34" s="51"/>
-      <c r="AA34" s="51"/>
-      <c r="AB34" s="53"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="51"/>
+      <c r="U34" s="50"/>
+      <c r="V34" s="50"/>
+      <c r="W34" s="50"/>
+      <c r="X34" s="50"/>
+      <c r="Y34" s="50"/>
+      <c r="Z34" s="50"/>
+      <c r="AA34" s="50"/>
+      <c r="AB34" s="52"/>
       <c r="AC34" s="44"/>
     </row>
     <row r="35" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="50"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="51"/>
-      <c r="V35" s="51"/>
-      <c r="W35" s="51"/>
-      <c r="X35" s="51"/>
-      <c r="Y35" s="51"/>
-      <c r="Z35" s="51"/>
-      <c r="AA35" s="51"/>
-      <c r="AB35" s="53"/>
+        <v>1</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="50"/>
+      <c r="V35" s="50"/>
+      <c r="W35" s="50"/>
+      <c r="X35" s="50">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="50"/>
+      <c r="Z35" s="50"/>
+      <c r="AA35" s="50"/>
+      <c r="AB35" s="52"/>
       <c r="AC35" s="44"/>
     </row>
     <row r="36" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3597,35 +3437,35 @@
         <v>1</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="52"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="50"/>
-      <c r="O36" s="50">
-        <v>1</v>
-      </c>
-      <c r="P36" s="50"/>
-      <c r="Q36" s="50"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="50"/>
-      <c r="T36" s="52"/>
-      <c r="U36" s="51"/>
-      <c r="V36" s="51"/>
-      <c r="W36" s="51"/>
-      <c r="X36" s="51"/>
-      <c r="Y36" s="51"/>
-      <c r="Z36" s="51"/>
-      <c r="AA36" s="51"/>
-      <c r="AB36" s="53"/>
+        <v>104</v>
+      </c>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="50"/>
+      <c r="V36" s="50"/>
+      <c r="W36" s="50"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="50"/>
+      <c r="Z36" s="50"/>
+      <c r="AA36" s="50"/>
+      <c r="AB36" s="52">
+        <v>1</v>
+      </c>
       <c r="AC36" s="44"/>
     </row>
     <row r="37" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3634,35 +3474,35 @@
         <v>1</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="52"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="50">
-        <v>1</v>
-      </c>
-      <c r="O37" s="50"/>
-      <c r="P37" s="50"/>
-      <c r="Q37" s="50"/>
-      <c r="R37" s="50"/>
-      <c r="S37" s="50"/>
-      <c r="T37" s="52"/>
-      <c r="U37" s="51"/>
-      <c r="V37" s="51"/>
-      <c r="W37" s="51"/>
-      <c r="X37" s="51"/>
-      <c r="Y37" s="51"/>
-      <c r="Z37" s="51"/>
-      <c r="AA37" s="51"/>
-      <c r="AB37" s="53"/>
+        <v>105</v>
+      </c>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="50"/>
+      <c r="V37" s="50"/>
+      <c r="W37" s="50"/>
+      <c r="X37" s="50"/>
+      <c r="Y37" s="50"/>
+      <c r="Z37" s="50"/>
+      <c r="AA37" s="50">
+        <v>1</v>
+      </c>
+      <c r="AB37" s="52"/>
       <c r="AC37" s="44"/>
     </row>
     <row r="38" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3670,31 +3510,34 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="52"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="50"/>
-      <c r="S38" s="50"/>
-      <c r="T38" s="52"/>
-      <c r="U38" s="51"/>
-      <c r="V38" s="51"/>
-      <c r="W38" s="51"/>
-      <c r="X38" s="51"/>
-      <c r="Y38" s="51"/>
-      <c r="Z38" s="51"/>
-      <c r="AA38" s="51"/>
-      <c r="AB38" s="53"/>
+      <c r="B38" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="51"/>
+      <c r="U38" s="50"/>
+      <c r="V38" s="50"/>
+      <c r="W38" s="50"/>
+      <c r="X38" s="50"/>
+      <c r="Y38" s="50"/>
+      <c r="Z38" s="50"/>
+      <c r="AA38" s="50"/>
+      <c r="AB38" s="52"/>
       <c r="AC38" s="44"/>
     </row>
     <row r="39" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3702,31 +3545,31 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="50"/>
-      <c r="R39" s="50"/>
-      <c r="S39" s="50"/>
-      <c r="T39" s="52"/>
-      <c r="U39" s="51"/>
-      <c r="V39" s="51"/>
-      <c r="W39" s="51"/>
-      <c r="X39" s="51"/>
-      <c r="Y39" s="51"/>
-      <c r="Z39" s="51"/>
-      <c r="AA39" s="51"/>
-      <c r="AB39" s="53"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="50"/>
+      <c r="V39" s="50"/>
+      <c r="W39" s="50"/>
+      <c r="X39" s="50"/>
+      <c r="Y39" s="50"/>
+      <c r="Z39" s="50"/>
+      <c r="AA39" s="50"/>
+      <c r="AB39" s="52"/>
       <c r="AC39" s="44"/>
     </row>
     <row r="40" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3737,33 +3580,33 @@
       <c r="B40" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="50"/>
-      <c r="R40" s="50"/>
-      <c r="S40" s="50"/>
-      <c r="T40" s="52"/>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51">
-        <v>1</v>
-      </c>
-      <c r="Y40" s="51"/>
-      <c r="Z40" s="51"/>
-      <c r="AA40" s="51"/>
-      <c r="AB40" s="53"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="51"/>
+      <c r="U40" s="50"/>
+      <c r="V40" s="50"/>
+      <c r="W40" s="50">
+        <v>1</v>
+      </c>
+      <c r="X40" s="50"/>
+      <c r="Y40" s="50"/>
+      <c r="Z40" s="50"/>
+      <c r="AA40" s="50"/>
+      <c r="AB40" s="52"/>
       <c r="AC40" s="44"/>
     </row>
     <row r="41" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -3771,179 +3614,159 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="52"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="50"/>
-      <c r="O41" s="50"/>
-      <c r="P41" s="50"/>
-      <c r="Q41" s="50"/>
-      <c r="R41" s="50"/>
-      <c r="S41" s="50"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="51"/>
-      <c r="V41" s="51"/>
-      <c r="W41" s="51"/>
-      <c r="X41" s="51"/>
-      <c r="Y41" s="51"/>
-      <c r="Z41" s="51"/>
-      <c r="AA41" s="51"/>
-      <c r="AB41" s="53"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="51"/>
+      <c r="U41" s="50"/>
+      <c r="V41" s="50"/>
+      <c r="W41" s="50"/>
+      <c r="X41" s="50"/>
+      <c r="Y41" s="50"/>
+      <c r="Z41" s="50"/>
+      <c r="AA41" s="50"/>
+      <c r="AB41" s="52"/>
       <c r="AC41" s="44"/>
     </row>
     <row r="42" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B42" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="47"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="52"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="50"/>
-      <c r="S42" s="50">
-        <v>1</v>
-      </c>
-      <c r="T42" s="52"/>
-      <c r="U42" s="51"/>
-      <c r="V42" s="51"/>
-      <c r="W42" s="51"/>
-      <c r="X42" s="51"/>
-      <c r="Y42" s="51"/>
-      <c r="Z42" s="51"/>
-      <c r="AA42" s="51"/>
-      <c r="AB42" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="51"/>
+      <c r="U42" s="50"/>
+      <c r="V42" s="50"/>
+      <c r="W42" s="50"/>
+      <c r="X42" s="50"/>
+      <c r="Y42" s="50"/>
+      <c r="Z42" s="50"/>
+      <c r="AA42" s="50"/>
+      <c r="AB42" s="52"/>
       <c r="AC42" s="44"/>
     </row>
     <row r="43" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="52"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="50"/>
-      <c r="R43" s="50">
-        <v>1</v>
-      </c>
-      <c r="S43" s="50"/>
-      <c r="T43" s="52"/>
-      <c r="U43" s="51"/>
-      <c r="V43" s="51"/>
-      <c r="W43" s="51"/>
-      <c r="X43" s="51"/>
-      <c r="Y43" s="51"/>
-      <c r="Z43" s="51"/>
-      <c r="AA43" s="51"/>
-      <c r="AB43" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="49"/>
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="51"/>
+      <c r="U43" s="50"/>
+      <c r="V43" s="50"/>
+      <c r="W43" s="50"/>
+      <c r="X43" s="50"/>
+      <c r="Y43" s="50"/>
+      <c r="Z43" s="50"/>
+      <c r="AA43" s="50"/>
+      <c r="AB43" s="52"/>
       <c r="AC43" s="44"/>
     </row>
     <row r="44" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="52"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50">
-        <v>1</v>
-      </c>
-      <c r="R44" s="50"/>
-      <c r="S44" s="50"/>
-      <c r="T44" s="52"/>
-      <c r="U44" s="51"/>
-      <c r="V44" s="51"/>
-      <c r="W44" s="51"/>
-      <c r="X44" s="51"/>
-      <c r="Y44" s="51"/>
-      <c r="Z44" s="51"/>
-      <c r="AA44" s="51"/>
-      <c r="AB44" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="49"/>
+      <c r="T44" s="51"/>
+      <c r="U44" s="50"/>
+      <c r="V44" s="50"/>
+      <c r="W44" s="50"/>
+      <c r="X44" s="50"/>
+      <c r="Y44" s="50"/>
+      <c r="Z44" s="50"/>
+      <c r="AA44" s="50"/>
+      <c r="AB44" s="52"/>
       <c r="AC44" s="44"/>
     </row>
     <row r="45" spans="1:29" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="52"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="50"/>
-      <c r="P45" s="50">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="50"/>
-      <c r="R45" s="50"/>
-      <c r="S45" s="50"/>
-      <c r="T45" s="52"/>
-      <c r="U45" s="51"/>
-      <c r="V45" s="51"/>
-      <c r="W45" s="51"/>
-      <c r="X45" s="51"/>
-      <c r="Y45" s="51"/>
-      <c r="Z45" s="51"/>
-      <c r="AA45" s="51"/>
-      <c r="AB45" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="49"/>
+      <c r="R45" s="49"/>
+      <c r="S45" s="49"/>
+      <c r="T45" s="51"/>
+      <c r="U45" s="50"/>
+      <c r="V45" s="50"/>
+      <c r="W45" s="50"/>
+      <c r="X45" s="50"/>
+      <c r="Y45" s="50"/>
+      <c r="Z45" s="50"/>
+      <c r="AA45" s="50"/>
+      <c r="AB45" s="52"/>
       <c r="AC45" s="44"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.15">
@@ -3951,68 +3774,64 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="54"/>
-      <c r="K46" s="54"/>
-      <c r="L46" s="55"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="57"/>
-      <c r="O46" s="57"/>
-      <c r="P46" s="57"/>
-      <c r="Q46" s="57"/>
-      <c r="R46" s="57"/>
-      <c r="S46" s="57"/>
-      <c r="T46" s="55"/>
-      <c r="U46" s="58"/>
-      <c r="V46" s="58"/>
-      <c r="W46" s="58"/>
-      <c r="X46" s="58"/>
-      <c r="Y46" s="58"/>
-      <c r="Z46" s="58"/>
-      <c r="AA46" s="58"/>
-      <c r="AB46" s="59"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="54"/>
+      <c r="M46" s="55"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
+      <c r="T46" s="54"/>
+      <c r="U46" s="57"/>
+      <c r="V46" s="57"/>
+      <c r="W46" s="57"/>
+      <c r="X46" s="57"/>
+      <c r="Y46" s="57"/>
+      <c r="Z46" s="57"/>
+      <c r="AA46" s="57"/>
+      <c r="AB46" s="58"/>
       <c r="AC46" s="10"/>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A47">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B47" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54">
-        <v>1</v>
-      </c>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="55"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="57"/>
-      <c r="O47" s="57"/>
-      <c r="P47" s="57"/>
-      <c r="Q47" s="57"/>
-      <c r="R47" s="57"/>
-      <c r="S47" s="57"/>
-      <c r="T47" s="55"/>
-      <c r="U47" s="58"/>
-      <c r="V47" s="58"/>
-      <c r="W47" s="58"/>
-      <c r="X47" s="58"/>
-      <c r="Y47" s="58"/>
-      <c r="Z47" s="58"/>
-      <c r="AA47" s="58"/>
-      <c r="AB47" s="59"/>
+        <v>0</v>
+      </c>
+      <c r="B47" s="33"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="55"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="56"/>
+      <c r="Q47" s="56"/>
+      <c r="R47" s="56"/>
+      <c r="S47" s="56"/>
+      <c r="T47" s="54"/>
+      <c r="U47" s="57"/>
+      <c r="V47" s="57"/>
+      <c r="W47" s="57"/>
+      <c r="X47" s="57"/>
+      <c r="Y47" s="57"/>
+      <c r="Z47" s="57"/>
+      <c r="AA47" s="57"/>
+      <c r="AB47" s="58"/>
       <c r="AC47" s="10"/>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.15">
@@ -4020,31 +3839,31 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D48" s="54"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="54"/>
-      <c r="G48" s="54"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="54"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="56"/>
-      <c r="N48" s="57"/>
-      <c r="O48" s="57"/>
-      <c r="P48" s="57"/>
-      <c r="Q48" s="57"/>
-      <c r="R48" s="57"/>
-      <c r="S48" s="57"/>
-      <c r="T48" s="55"/>
-      <c r="U48" s="58"/>
-      <c r="V48" s="58"/>
-      <c r="W48" s="58"/>
-      <c r="X48" s="58"/>
-      <c r="Y48" s="58"/>
-      <c r="Z48" s="58"/>
-      <c r="AA48" s="58"/>
-      <c r="AB48" s="59"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="54"/>
+      <c r="M48" s="55"/>
+      <c r="N48" s="56"/>
+      <c r="O48" s="56"/>
+      <c r="P48" s="56"/>
+      <c r="Q48" s="56"/>
+      <c r="R48" s="56"/>
+      <c r="S48" s="56"/>
+      <c r="T48" s="54"/>
+      <c r="U48" s="57"/>
+      <c r="V48" s="57"/>
+      <c r="W48" s="57"/>
+      <c r="X48" s="57"/>
+      <c r="Y48" s="57"/>
+      <c r="Z48" s="57"/>
+      <c r="AA48" s="57"/>
+      <c r="AB48" s="58"/>
       <c r="AC48" s="10"/>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.15">
@@ -4052,31 +3871,31 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="54"/>
-      <c r="J49" s="54"/>
-      <c r="K49" s="54"/>
-      <c r="L49" s="55"/>
-      <c r="M49" s="56"/>
-      <c r="N49" s="57"/>
-      <c r="O49" s="57"/>
-      <c r="P49" s="57"/>
-      <c r="Q49" s="57"/>
-      <c r="R49" s="57"/>
-      <c r="S49" s="57"/>
-      <c r="T49" s="55"/>
-      <c r="U49" s="58"/>
-      <c r="V49" s="58"/>
-      <c r="W49" s="58"/>
-      <c r="X49" s="58"/>
-      <c r="Y49" s="58"/>
-      <c r="Z49" s="58"/>
-      <c r="AA49" s="58"/>
-      <c r="AB49" s="59"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="53"/>
+      <c r="L49" s="54"/>
+      <c r="M49" s="55"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="56"/>
+      <c r="R49" s="56"/>
+      <c r="S49" s="56"/>
+      <c r="T49" s="54"/>
+      <c r="U49" s="57"/>
+      <c r="V49" s="57"/>
+      <c r="W49" s="57"/>
+      <c r="X49" s="57"/>
+      <c r="Y49" s="57"/>
+      <c r="Z49" s="57"/>
+      <c r="AA49" s="57"/>
+      <c r="AB49" s="58"/>
       <c r="AC49" s="10"/>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.15">
@@ -4084,31 +3903,31 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="54"/>
-      <c r="I50" s="54"/>
-      <c r="J50" s="54"/>
-      <c r="K50" s="54"/>
-      <c r="L50" s="55"/>
-      <c r="M50" s="56"/>
-      <c r="N50" s="57"/>
-      <c r="O50" s="57"/>
-      <c r="P50" s="57"/>
-      <c r="Q50" s="57"/>
-      <c r="R50" s="57"/>
-      <c r="S50" s="57"/>
-      <c r="T50" s="55"/>
-      <c r="U50" s="58"/>
-      <c r="V50" s="58"/>
-      <c r="W50" s="58"/>
-      <c r="X50" s="58"/>
-      <c r="Y50" s="58"/>
-      <c r="Z50" s="58"/>
-      <c r="AA50" s="58"/>
-      <c r="AB50" s="59"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="54"/>
+      <c r="M50" s="55"/>
+      <c r="N50" s="56"/>
+      <c r="O50" s="56"/>
+      <c r="P50" s="56"/>
+      <c r="Q50" s="56"/>
+      <c r="R50" s="56"/>
+      <c r="S50" s="56"/>
+      <c r="T50" s="54"/>
+      <c r="U50" s="57"/>
+      <c r="V50" s="57"/>
+      <c r="W50" s="57"/>
+      <c r="X50" s="57"/>
+      <c r="Y50" s="57"/>
+      <c r="Z50" s="57"/>
+      <c r="AA50" s="57"/>
+      <c r="AB50" s="58"/>
       <c r="AC50" s="10"/>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.15">
@@ -4970,7 +4789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -4985,7 +4804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AM67"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
@@ -6682,7 +6501,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
@@ -7660,7 +7479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE79"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
@@ -8147,7 +7966,7 @@
         <v>LAMPEEIN</v>
       </c>
       <c r="AE11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.15">
@@ -8189,7 +8008,7 @@
         <v>LAMPEAUS</v>
       </c>
       <c r="AE12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.15">
@@ -8261,7 +8080,7 @@
         <v>OFENEIN</v>
       </c>
       <c r="AE14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.15">
@@ -8303,7 +8122,7 @@
         <v>OFENAUS</v>
       </c>
       <c r="AE15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.15">
@@ -9181,7 +9000,7 @@
         <v>ADC Vorlauf</v>
       </c>
       <c r="AE42" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.15">
@@ -9223,7 +9042,7 @@
         <v>ADC Rücklauf</v>
       </c>
       <c r="AE43" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.15">
@@ -9265,7 +9084,7 @@
         <v>ADC Aussen</v>
       </c>
       <c r="AE44" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.15">
@@ -9307,7 +9126,7 @@
         <v>ADC Tastatur</v>
       </c>
       <c r="AE45" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.15">
@@ -10316,7 +10135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE80"/>
   <sheetViews>
     <sheetView topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
@@ -10327,7 +10146,7 @@
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="54" customWidth="1"/>
     <col min="4" max="11" width="2.5" style="2" customWidth="1"/>
     <col min="12" max="12" width="2.5" customWidth="1"/>
     <col min="13" max="19" width="2.5" style="3" customWidth="1"/>
@@ -10339,7 +10158,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B1" s="17"/>
     </row>
@@ -10563,7 +10382,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C6" s="61"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="5">
         <v>7</v>
       </c>
@@ -10804,7 +10623,7 @@
         <v>LAMPEEIN</v>
       </c>
       <c r="AE11" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.15">
@@ -10846,7 +10665,7 @@
         <v>LAMPEAUS</v>
       </c>
       <c r="AE12" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.15">
@@ -10918,7 +10737,7 @@
         <v>OFENEIN</v>
       </c>
       <c r="AE14" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.15">
@@ -10960,7 +10779,7 @@
         <v>OFENAUS</v>
       </c>
       <c r="AE15" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.15">
@@ -10999,7 +10818,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -11034,7 +10853,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -11069,7 +10888,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -11104,7 +10923,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -11432,7 +11251,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -11657,8 +11476,8 @@
       <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="55" t="s">
-        <v>109</v>
+      <c r="C37" s="54" t="s">
+        <v>74</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -11695,8 +11514,8 @@
       <c r="B38" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="55" t="s">
-        <v>110</v>
+      <c r="C38" s="54" t="s">
+        <v>75</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -11856,7 +11675,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -11917,7 +11736,7 @@
         <v>0</v>
       </c>
       <c r="AE44" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.15">
@@ -11957,7 +11776,7 @@
         <v>ADC Aussen</v>
       </c>
       <c r="AE45" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.15">
@@ -11999,7 +11818,7 @@
         <v>ADC Tastatur</v>
       </c>
       <c r="AE46" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.15">
@@ -12068,10 +11887,10 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="55" t="s">
-        <v>107</v>
+        <v>71</v>
+      </c>
+      <c r="C49" s="54" t="s">
+        <v>72</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -12104,10 +11923,10 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50" s="55" t="s">
-        <v>108</v>
+        <v>71</v>
+      </c>
+      <c r="C50" s="54" t="s">
+        <v>73</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -12200,7 +12019,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -13029,7 +12848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BV132"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -13041,7 +12860,7 @@
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="55" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="54" customWidth="1"/>
     <col min="4" max="12" width="2.33203125" customWidth="1"/>
     <col min="13" max="20" width="2.33203125" style="2" customWidth="1"/>
     <col min="21" max="22" width="2.33203125" customWidth="1"/>
@@ -13053,60 +12872,60 @@
   <sheetData>
     <row r="1" spans="1:39" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B1" s="17"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="O1" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="P1" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC1" s="66" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH1" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC1" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH1" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
@@ -13389,7 +13208,7 @@
       </c>
     </row>
     <row r="6" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C6" s="61"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="1">
         <v>7</v>
       </c>
@@ -13614,8 +13433,8 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="55" t="s">
-        <v>105</v>
+      <c r="C10" s="54" t="s">
+        <v>70</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
@@ -13661,8 +13480,8 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="55" t="s">
-        <v>120</v>
+      <c r="C11" s="54" t="s">
+        <v>85</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
@@ -13706,7 +13525,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
@@ -13867,7 +13686,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="D16" s="29">
         <v>1</v>
@@ -13952,7 +13771,7 @@
       <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
@@ -14205,7 +14024,7 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
@@ -14247,7 +14066,7 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
@@ -14289,7 +14108,7 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
@@ -14453,7 +14272,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
@@ -14541,7 +14360,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
@@ -14752,7 +14571,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
@@ -14835,7 +14654,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29">
@@ -15290,7 +15109,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29"/>
@@ -15495,7 +15314,7 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
@@ -15539,7 +15358,7 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="29"/>
@@ -15661,7 +15480,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29"/>
@@ -15783,7 +15602,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29"/>
@@ -15827,7 +15646,7 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29"/>
@@ -15947,7 +15766,7 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29"/>
@@ -15991,7 +15810,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29"/>
@@ -16035,7 +15854,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29"/>
@@ -16079,7 +15898,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29"/>
@@ -18531,7 +18350,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BD72"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
@@ -18542,7 +18361,7 @@
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.83203125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" style="54" customWidth="1"/>
     <col min="4" max="11" width="2.5" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="2.5" customWidth="1"/>
     <col min="13" max="20" width="2.5" style="2" customWidth="1"/>
@@ -18555,7 +18374,7 @@
   <sheetData>
     <row r="1" spans="1:56" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="B1" s="17"/>
       <c r="D1" s="1"/>
@@ -18850,7 +18669,7 @@
     <row r="6" spans="1:56" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6"/>
       <c r="B6"/>
-      <c r="C6" s="55"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="29">
         <v>7</v>
       </c>
@@ -18925,7 +18744,7 @@
       <c r="AC6" s="6">
         <v>0</v>
       </c>
-      <c r="AD6" s="60"/>
+      <c r="AD6" s="59"/>
       <c r="AE6" s="7">
         <v>7</v>
       </c>
@@ -19017,10 +18836,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>102</v>
+        <v>65</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -19064,7 +18883,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
@@ -19516,7 +19335,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
@@ -19560,7 +19379,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
@@ -19604,10 +19423,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="55" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>68</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
@@ -19651,7 +19470,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
@@ -19857,10 +19676,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>105</v>
+        <v>69</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>70</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
@@ -20221,10 +20040,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="55" t="s">
-        <v>107</v>
+        <v>71</v>
+      </c>
+      <c r="C37" s="54" t="s">
+        <v>72</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
@@ -20264,10 +20083,10 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="55" t="s">
-        <v>108</v>
+        <v>71</v>
+      </c>
+      <c r="C38" s="54" t="s">
+        <v>73</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
@@ -20467,7 +20286,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
@@ -20509,7 +20328,7 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
@@ -20629,7 +20448,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
@@ -21455,7 +21274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BD72"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
@@ -21849,7 +21668,7 @@
       <c r="AC6" s="6">
         <v>0</v>
       </c>
-      <c r="AD6" s="60"/>
+      <c r="AD6" s="59"/>
       <c r="AE6" s="7">
         <v>7</v>
       </c>
@@ -23042,7 +22861,7 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
@@ -23086,7 +22905,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
@@ -23130,7 +22949,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
@@ -23209,7 +23028,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
@@ -23253,7 +23072,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
@@ -23297,7 +23116,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29"/>
@@ -23380,7 +23199,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
@@ -23422,7 +23241,7 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
@@ -23542,7 +23361,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
@@ -24369,7 +24188,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AM79"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -27484,7 +27303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AE67"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
@@ -28726,7 +28545,7 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -28762,7 +28581,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -28798,7 +28617,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -28834,7 +28653,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>

</xml_diff>